<commit_message>
example 05-06 declarations in a template
</commit_message>
<xml_diff>
--- a/src/demo/zxxt_05_excel_xlsx.w3mi.data.xlsx
+++ b/src/demo/zxxt_05_excel_xlsx.w3mi.data.xlsx
@@ -1,25 +1,299 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="19001"/>
-  <workbookPr defaultThemeVersion="166925"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
+  <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\IBM_ADMIN\Desktop\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Users\MoldaB\Desktop\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="24000" windowHeight="9660" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="24000" windowHeight="9660"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="No group" sheetId="2" r:id="rId1"/>
+    <sheet name="With Total" sheetId="4" r:id="rId2"/>
+    <sheet name="group by 1 field" sheetId="1" r:id="rId3"/>
+    <sheet name="group by 1 field(level orders)" sheetId="5" r:id="rId4"/>
+    <sheet name="Different format for levels" sheetId="6" r:id="rId5"/>
   </sheets>
-  <calcPr calcId="0"/>
+  <calcPr calcId="162913"/>
 </workbook>
 </file>
 
+<file path=xl/comments1.xml><?xml version="1.0" encoding="utf-8"?>
+<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <authors>
+    <author>Moldabayev, Birzhan</author>
+  </authors>
+  <commentList>
+    <comment ref="A1" authorId="0" shapeId="0">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+            <charset val="204"/>
+          </rPr>
+          <t>Empty group means:
+0</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+            <charset val="204"/>
+          </rPr>
+          <t xml:space="preserve"> - Total
+</t>
+        </r>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+            <charset val="204"/>
+          </rPr>
+          <t xml:space="preserve">1 </t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+            <charset val="204"/>
+          </rPr>
+          <t>- Data level</t>
+        </r>
+      </text>
+    </comment>
+  </commentList>
+</comments>
+</file>
+
+<file path=xl/comments2.xml><?xml version="1.0" encoding="utf-8"?>
+<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <authors>
+    <author>Moldabayev, Birzhan</author>
+  </authors>
+  <commentList>
+    <comment ref="A1" authorId="0" shapeId="0">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+            <charset val="204"/>
+          </rPr>
+          <t>Attention:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+            <charset val="204"/>
+          </rPr>
+          <t xml:space="preserve">
+Just type {R-T;group=GROUP} anywhere
+Or use in code zcl_xtt_replace_block=&gt;</t>
+        </r>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+            <charset val="204"/>
+          </rPr>
+          <t xml:space="preserve">tree_create
+@see </t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+            <charset val="204"/>
+          </rPr>
+          <t>Z_XTT_INDEX_EXA_05</t>
+        </r>
+      </text>
+    </comment>
+  </commentList>
+</comments>
+</file>
+
+<file path=xl/comments3.xml><?xml version="1.0" encoding="utf-8"?>
+<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <authors>
+    <author>Moldabayev, Birzhan</author>
+  </authors>
+  <commentList>
+    <comment ref="A1" authorId="0" shapeId="0">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+            <charset val="204"/>
+          </rPr>
+          <t>Attention:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+            <charset val="204"/>
+          </rPr>
+          <t xml:space="preserve">
+Just type {R-T;group=GROUP} anywhere
+Or use in code zcl_xtt_replace_block=&gt;</t>
+        </r>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+            <charset val="204"/>
+          </rPr>
+          <t xml:space="preserve">tree_create
+@see </t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+            <charset val="204"/>
+          </rPr>
+          <t>Z_XTT_INDEX_EXA_05</t>
+        </r>
+      </text>
+    </comment>
+  </commentList>
+</comments>
+</file>
+
+<file path=xl/comments4.xml><?xml version="1.0" encoding="utf-8"?>
+<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <authors>
+    <author>Moldabayev, Birzhan</author>
+  </authors>
+  <commentList>
+    <comment ref="A1" authorId="0" shapeId="0">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+            <charset val="204"/>
+          </rPr>
+          <t>Attention:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+            <charset val="204"/>
+          </rPr>
+          <t xml:space="preserve">
+Just type {R-T;group=GROUP} anywhere
+Or use in code zcl_xtt_replace_block=&gt;</t>
+        </r>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+            <charset val="204"/>
+          </rPr>
+          <t>tree_create</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+            <charset val="204"/>
+          </rPr>
+          <t xml:space="preserve">
+</t>
+        </r>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+            <charset val="204"/>
+          </rPr>
+          <t>@see</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+            <charset val="204"/>
+          </rPr>
+          <t xml:space="preserve"> Z_XTT_INDEX_EXA_05</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="D4" authorId="0" shapeId="0">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t>1 formula for level=1</t>
+        </r>
+      </text>
+    </comment>
+  </commentList>
+</comments>
+</file>
+
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="25" uniqueCount="19">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="118" uniqueCount="46">
   <si>
     <t>{R-TITLE}</t>
   </si>
@@ -45,9 +319,6 @@
     <t xml:space="preserve">Totals for all groups </t>
   </si>
   <si>
-    <t>Groups count {R-T-CH_COUNT}</t>
-  </si>
-  <si>
     <t>{R-T-SUM1}</t>
   </si>
   <si>
@@ -60,9 +331,6 @@
     <t xml:space="preserve">Sub totals of group {R-T-GROUP} </t>
   </si>
   <si>
-    <t>Sub items count {R-T-CH_COUNT}</t>
-  </si>
-  <si>
     <t>{R-T;level=1;top=}</t>
   </si>
   <si>
@@ -76,13 +344,100 @@
   </si>
   <si>
     <t>{R-T-GROUP}</t>
+  </si>
+  <si>
+    <t>{R-T;group=GROUP}</t>
+  </si>
+  <si>
+    <t>{R-T;group=}</t>
+  </si>
+  <si>
+    <t>{R-T;level=1}</t>
+  </si>
+  <si>
+    <t>{R-T-SUM1;func=SUM}</t>
+  </si>
+  <si>
+    <t>{R-T-SUM2;func=AVG}</t>
+  </si>
+  <si>
+    <t>Total count: {R-T-CAPTION;func=COUNT}</t>
+  </si>
+  <si>
+    <t>Levels=0,1,2</t>
+  </si>
+  <si>
+    <t>{R-T-SUM2;func=SUM}</t>
+  </si>
+  <si>
+    <t>Groups count {R-T-CAPTION;func=COUNT}</t>
+  </si>
+  <si>
+    <t>Sub items count {R-T-CAPTION;func=COUNT}</t>
+  </si>
+  <si>
+    <t>Level order does not matter</t>
+  </si>
+  <si>
+    <t>DEFAULT header (WHEN OTHERS)</t>
+  </si>
+  <si>
+    <t>Group {R-T-GROUP;func=FIRST}</t>
+  </si>
+  <si>
+    <t>{R-T;level=1;top=X;show_if=ROW-GROUP eq 'GRP B'}</t>
+  </si>
+  <si>
+    <t>Header for GROUP 'B' 2 rows</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Group {R-T-GROUP} </t>
+  </si>
+  <si>
+    <t>{R-T;level=1;top=X;show_if=( row-GROUP = 'C' OR ROW-group cp '*C' ) AND ROW-GROUP &lt;&gt; 'Z' }</t>
+  </si>
+  <si>
+    <t>Complex where with ()</t>
+  </si>
+  <si>
+    <t>{R-T;level=1;top=X;hide_if=row-GROUP = 'GRP D'}</t>
+  </si>
+  <si>
+    <t>Do not show header for 'D' group! (hide_if=)</t>
+  </si>
+  <si>
+    <t>The last level is hid</t>
+  </si>
+  <si>
+    <t>Footer is the same</t>
+  </si>
+  <si>
+    <t>End of {R-T-GROUP} sum for SUM1 &amp; SUM2</t>
+  </si>
+  <si>
+    <t>Average for SUM1 &amp; SUM2</t>
+  </si>
+  <si>
+    <t>{R-T-SUM1;func=AVG}</t>
+  </si>
+  <si>
+    <t>COUNT = {R-T-CAPTION;func=COUNT}</t>
+  </si>
+  <si>
+    <t>COUNT= {R-T-CAPTION}</t>
+  </si>
+  <si>
+    <t>Sub items count {R-T-CAPTION}</t>
+  </si>
+  <si>
+    <t>Groups count {R-T-CAPTION;func=COUNT} (level=0)</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="18" x14ac:knownFonts="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+  <fonts count="24" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color indexed="8"/>
@@ -234,8 +589,53 @@
       <charset val="204"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="9"/>
+      <color indexed="81"/>
+      <name val="Tahoma"/>
+      <family val="2"/>
+      <charset val="204"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="9"/>
+      <color indexed="81"/>
+      <name val="Tahoma"/>
+      <family val="2"/>
+      <charset val="204"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color indexed="8"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <charset val="204"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FFFF0000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <charset val="204"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFF0000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <charset val="204"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="9"/>
+      <color indexed="81"/>
+      <name val="Tahoma"/>
+      <charset val="1"/>
+    </font>
   </fonts>
-  <fills count="36">
+  <fills count="42">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -433,8 +833,44 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFF00"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.59999389629810485"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.59999389629810485"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.59999389629810485"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="-0.249977111117893"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.79998168889431442"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="20">
+  <borders count="27">
     <border>
       <left/>
       <right/>
@@ -613,13 +1049,58 @@
         <color auto="1"/>
       </left>
       <right/>
+      <top style="medium">
+        <color auto="1"/>
+      </top>
+      <bottom style="medium">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="medium">
+        <color auto="1"/>
+      </top>
+      <bottom style="medium">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color auto="1"/>
+      </left>
+      <right style="thin">
+        <color auto="1"/>
+      </right>
+      <top style="thin">
+        <color auto="1"/>
+      </top>
+      <bottom style="thin">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color auto="1"/>
+      </left>
+      <right style="thin">
+        <color auto="1"/>
+      </right>
       <top/>
-      <bottom/>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right style="medium">
+      <bottom style="thin">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color auto="1"/>
+      </left>
+      <right style="thin">
         <color auto="1"/>
       </right>
       <top/>
@@ -627,42 +1108,84 @@
       <diagonal/>
     </border>
     <border>
-      <left style="medium">
-        <color auto="1"/>
+      <left style="thin">
+        <color indexed="64"/>
       </left>
       <right/>
-      <top style="medium">
-        <color auto="1"/>
+      <top style="thin">
+        <color indexed="64"/>
       </top>
-      <bottom style="medium">
-        <color auto="1"/>
+      <bottom style="thin">
+        <color indexed="64"/>
       </bottom>
       <diagonal/>
     </border>
     <border>
       <left/>
       <right/>
-      <top style="medium">
-        <color auto="1"/>
+      <top style="thin">
+        <color indexed="64"/>
       </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color auto="1"/>
+      </left>
+      <right/>
+      <top/>
       <bottom style="medium">
-        <color auto="1"/>
+        <color indexed="64"/>
       </bottom>
       <diagonal/>
     </border>
     <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="medium">
+        <color auto="1"/>
+      </right>
+      <top/>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
       <left style="thin">
-        <color auto="1"/>
+        <color indexed="64"/>
       </left>
       <right style="thin">
-        <color auto="1"/>
+        <color indexed="64"/>
       </right>
       <top style="thin">
-        <color auto="1"/>
+        <color indexed="64"/>
       </top>
-      <bottom style="thin">
-        <color auto="1"/>
-      </bottom>
+      <bottom/>
       <diagonal/>
     </border>
   </borders>
@@ -710,7 +1233,7 @@
     <xf numFmtId="0" fontId="1" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="20">
+  <cellXfs count="64">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment vertical="center"/>
@@ -722,31 +1245,41 @@
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="34" borderId="15" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="35" borderId="15" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="34" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="35" borderId="16" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="4" fontId="0" fillId="34" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="4" fontId="0" fillId="34" borderId="16" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="35" borderId="17" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="35" borderId="18" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="4" fontId="0" fillId="35" borderId="18" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="4" fontId="0" fillId="35" borderId="16" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="4" fontId="0" fillId="35" borderId="11" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="4" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="17" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="17" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="4" fontId="0" fillId="0" borderId="17" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="36" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="18" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="18" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="4" fontId="0" fillId="0" borderId="18" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="19" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
@@ -756,6 +1289,69 @@
     <xf numFmtId="4" fontId="0" fillId="0" borderId="19" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="20" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="21" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="4" fontId="20" fillId="0" borderId="21" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="4" fontId="20" fillId="0" borderId="22" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="37" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="37" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="37" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="34" borderId="23" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="34" borderId="24" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="4" fontId="0" fillId="34" borderId="24" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="4" fontId="0" fillId="34" borderId="25" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="36" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="38" borderId="26" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="26" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="35" borderId="16" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="38" borderId="19" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="19" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="37" borderId="16" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="4" fontId="0" fillId="37" borderId="16" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="4" fontId="0" fillId="37" borderId="11" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="38" borderId="18" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="21" fillId="0" borderId="18" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="22" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="40" borderId="17" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="4" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="41" borderId="26" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="41" borderId="18" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="22" fillId="41" borderId="23" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="41" borderId="24" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="4" fontId="0" fillId="41" borderId="24" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="4" fontId="0" fillId="41" borderId="25" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" quotePrefix="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -764,6 +1360,27 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" quotePrefix="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="19" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="39" borderId="13" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="39" borderId="24" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="4" fontId="0" fillId="39" borderId="13" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="4" fontId="0" fillId="39" borderId="24" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="4" fontId="0" fillId="39" borderId="14" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="4" fontId="0" fillId="39" borderId="25" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="42">
@@ -1119,14 +1736,146 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="C1:F4"/>
+  <sheetViews>
+    <sheetView tabSelected="1" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
+      <selection activeCell="H1" sqref="H1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="3" max="3" width="46" customWidth="1"/>
+    <col min="4" max="4" width="41.85546875" customWidth="1"/>
+    <col min="5" max="6" width="33.42578125" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="3:6" x14ac:dyDescent="0.25">
+      <c r="C1" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="2" spans="3:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="3" spans="3:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="C3" s="17" t="s">
+        <v>1</v>
+      </c>
+      <c r="D3" s="17" t="s">
+        <v>2</v>
+      </c>
+      <c r="E3" s="17" t="s">
+        <v>3</v>
+      </c>
+      <c r="F3" s="17" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="4" spans="3:6" x14ac:dyDescent="0.25">
+      <c r="C4" s="14" t="s">
+        <v>15</v>
+      </c>
+      <c r="D4" s="15" t="s">
+        <v>16</v>
+      </c>
+      <c r="E4" s="16" t="s">
+        <v>8</v>
+      </c>
+      <c r="F4" s="16" t="s">
+        <v>9</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:F5"/>
+  <sheetViews>
+    <sheetView zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
+      <selection activeCell="G1" sqref="G1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="19.140625" customWidth="1"/>
+    <col min="3" max="3" width="46" customWidth="1"/>
+    <col min="4" max="4" width="41.85546875" customWidth="1"/>
+    <col min="5" max="6" width="33.42578125" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A1" s="13" t="s">
+        <v>18</v>
+      </c>
+      <c r="C1" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="3" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="C3" s="17" t="s">
+        <v>1</v>
+      </c>
+      <c r="D3" s="17" t="s">
+        <v>2</v>
+      </c>
+      <c r="E3" s="17" t="s">
+        <v>3</v>
+      </c>
+      <c r="F3" s="17" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>19</v>
+      </c>
+      <c r="C4" s="18" t="s">
+        <v>15</v>
+      </c>
+      <c r="D4" s="19" t="s">
+        <v>16</v>
+      </c>
+      <c r="E4" s="20" t="s">
+        <v>8</v>
+      </c>
+      <c r="F4" s="20" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6" s="21" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A5" s="21" t="s">
+        <v>5</v>
+      </c>
+      <c r="C5" s="22" t="s">
+        <v>22</v>
+      </c>
+      <c r="D5" s="23"/>
+      <c r="E5" s="24" t="s">
+        <v>20</v>
+      </c>
+      <c r="F5" s="25" t="s">
+        <v>21</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+  <legacyDrawing r:id="rId2"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr>
     <outlinePr summaryBelow="0"/>
   </sheetPr>
   <dimension ref="A1:F9"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="85" workbookViewId="0">
-      <selection activeCell="F1" sqref="F1"/>
+    <sheetView zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
+      <selection activeCell="G1" sqref="G1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" customHeight="1" outlineLevelRow="1" x14ac:dyDescent="0.25"/>
@@ -1139,11 +1888,17 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A1" s="13" t="s">
+        <v>17</v>
+      </c>
       <c r="B1" s="1" t="s">
         <v>0</v>
       </c>
     </row>
     <row r="2" spans="1:6" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A2" t="s">
+        <v>23</v>
+      </c>
       <c r="B2" s="1"/>
     </row>
     <row r="3" spans="1:6" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
@@ -1164,79 +1919,79 @@
       <c r="A4" s="4" t="s">
         <v>5</v>
       </c>
-      <c r="B4" s="17" t="s">
+      <c r="B4" s="54" t="s">
         <v>6</v>
       </c>
-      <c r="C4" s="18"/>
-      <c r="D4" s="18"/>
-      <c r="E4" s="19"/>
+      <c r="C4" s="55"/>
+      <c r="D4" s="55"/>
+      <c r="E4" s="56"/>
       <c r="F4" s="4"/>
     </row>
     <row r="5" spans="1:6" ht="24.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
         <v>5</v>
       </c>
-      <c r="B5" s="5" t="s">
+      <c r="B5" s="29" t="s">
         <v>7</v>
       </c>
-      <c r="C5" s="6" t="s">
-        <v>8</v>
-      </c>
-      <c r="D5" s="7" t="s">
-        <v>9</v>
-      </c>
-      <c r="E5" s="8" t="s">
-        <v>10</v>
+      <c r="C5" s="30" t="s">
+        <v>25</v>
+      </c>
+      <c r="D5" s="31" t="s">
+        <v>20</v>
+      </c>
+      <c r="E5" s="32" t="s">
+        <v>24</v>
       </c>
     </row>
     <row r="6" spans="1:6" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
+        <v>10</v>
+      </c>
+      <c r="B6" s="5" t="s">
         <v>11</v>
       </c>
-      <c r="B6" s="9" t="s">
-        <v>12</v>
-      </c>
-      <c r="C6" s="10" t="s">
-        <v>13</v>
-      </c>
-      <c r="D6" s="11" t="s">
-        <v>9</v>
-      </c>
-      <c r="E6" s="12" t="s">
-        <v>10</v>
+      <c r="C6" s="6" t="s">
+        <v>26</v>
+      </c>
+      <c r="D6" s="7" t="s">
+        <v>20</v>
+      </c>
+      <c r="E6" s="8" t="s">
+        <v>24</v>
       </c>
     </row>
     <row r="7" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
+        <v>12</v>
+      </c>
+      <c r="B7" t="s">
+        <v>13</v>
+      </c>
+      <c r="D7" s="9"/>
+      <c r="E7" s="9"/>
+    </row>
+    <row r="8" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A8" t="s">
+        <v>12</v>
+      </c>
+      <c r="D8" s="9"/>
+      <c r="E8" s="9"/>
+    </row>
+    <row r="9" spans="1:6" ht="15.75" customHeight="1" outlineLevel="1" x14ac:dyDescent="0.25">
+      <c r="A9" t="s">
         <v>14</v>
       </c>
-      <c r="B7" t="s">
+      <c r="B9" s="10" t="s">
         <v>15</v>
       </c>
-      <c r="D7" s="13"/>
-      <c r="E7" s="13"/>
-    </row>
-    <row r="8" spans="1:6" ht="15.75" customHeight="1" collapsed="1" x14ac:dyDescent="0.25">
-      <c r="A8" t="s">
-        <v>14</v>
-      </c>
-      <c r="D8" s="13"/>
-      <c r="E8" s="13"/>
-    </row>
-    <row r="9" spans="1:6" ht="15.75" hidden="1" customHeight="1" outlineLevel="1" x14ac:dyDescent="0.25">
-      <c r="A9" t="s">
+      <c r="C9" s="11" t="s">
         <v>16</v>
       </c>
-      <c r="B9" s="14" t="s">
-        <v>17</v>
-      </c>
-      <c r="C9" s="15" t="s">
-        <v>18</v>
-      </c>
-      <c r="D9" s="16" t="s">
-        <v>9</v>
-      </c>
-      <c r="E9" s="16" t="s">
+      <c r="D9" s="12" t="s">
+        <v>8</v>
+      </c>
+      <c r="E9" s="12" t="s">
         <v>9</v>
       </c>
     </row>
@@ -1245,6 +2000,341 @@
     <mergeCell ref="B4:E4"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+  <legacyDrawing r:id="rId2"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <sheetPr>
+    <outlinePr summaryBelow="0"/>
+  </sheetPr>
+  <dimension ref="A1:E9"/>
+  <sheetViews>
+    <sheetView zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
+      <selection activeCell="C4" sqref="C4"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" outlineLevelRow="1" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="22" customWidth="1"/>
+    <col min="2" max="2" width="46" customWidth="1"/>
+    <col min="3" max="3" width="41.85546875" customWidth="1"/>
+    <col min="4" max="5" width="33.42578125" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A1" s="13" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="3" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A3" s="26" t="s">
+        <v>27</v>
+      </c>
+      <c r="B3" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="C3" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="D3" s="3" t="s">
+        <v>3</v>
+      </c>
+      <c r="E3" s="3" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" ht="15.75" collapsed="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A4" s="27" t="s">
+        <v>10</v>
+      </c>
+      <c r="B4" s="5" t="s">
+        <v>11</v>
+      </c>
+      <c r="C4" s="6" t="s">
+        <v>26</v>
+      </c>
+      <c r="D4" s="7" t="s">
+        <v>20</v>
+      </c>
+      <c r="E4" s="8" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
+      <c r="A5" s="27" t="s">
+        <v>14</v>
+      </c>
+      <c r="B5" s="10" t="s">
+        <v>15</v>
+      </c>
+      <c r="C5" s="11" t="s">
+        <v>16</v>
+      </c>
+      <c r="D5" s="12" t="s">
+        <v>8</v>
+      </c>
+      <c r="E5" s="12" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A6" s="27" t="s">
+        <v>12</v>
+      </c>
+      <c r="B6" t="s">
+        <v>13</v>
+      </c>
+      <c r="D6" s="9"/>
+      <c r="E6" s="9"/>
+    </row>
+    <row r="7" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A7" s="27" t="s">
+        <v>12</v>
+      </c>
+      <c r="D7" s="9"/>
+      <c r="E7" s="9"/>
+    </row>
+    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A8" s="28" t="s">
+        <v>5</v>
+      </c>
+      <c r="B8" s="54" t="s">
+        <v>6</v>
+      </c>
+      <c r="C8" s="55"/>
+      <c r="D8" s="55"/>
+      <c r="E8" s="56"/>
+    </row>
+    <row r="9" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A9" s="27" t="s">
+        <v>5</v>
+      </c>
+      <c r="B9" s="29" t="s">
+        <v>7</v>
+      </c>
+      <c r="C9" s="30" t="s">
+        <v>25</v>
+      </c>
+      <c r="D9" s="31" t="s">
+        <v>20</v>
+      </c>
+      <c r="E9" s="32" t="s">
+        <v>24</v>
+      </c>
+    </row>
+  </sheetData>
+  <mergeCells count="1">
+    <mergeCell ref="B8:E8"/>
+  </mergeCells>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <legacyDrawing r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <sheetPr>
+    <outlinePr summaryBelow="0"/>
+  </sheetPr>
+  <dimension ref="A1:G13"/>
+  <sheetViews>
+    <sheetView zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="G1" sqref="G1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" customHeight="1" outlineLevelRow="1" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="20.7109375" customWidth="1"/>
+    <col min="2" max="2" width="42.5703125" customWidth="1"/>
+    <col min="3" max="3" width="46" customWidth="1"/>
+    <col min="4" max="4" width="41.85546875" customWidth="1"/>
+    <col min="5" max="7" width="33.42578125" customWidth="1"/>
+    <col min="8" max="8" width="30.42578125" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A1" s="33" t="s">
+        <v>17</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="2" spans="1:7" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="C2" s="1"/>
+    </row>
+    <row r="3" spans="1:7" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="C3" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="D3" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="E3" s="3" t="s">
+        <v>3</v>
+      </c>
+      <c r="F3" s="3" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="4" spans="1:7" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A4" s="34" t="s">
+        <v>10</v>
+      </c>
+      <c r="B4" s="35" t="s">
+        <v>28</v>
+      </c>
+      <c r="C4" s="36" t="s">
+        <v>29</v>
+      </c>
+      <c r="D4" s="36" t="s">
+        <v>42</v>
+      </c>
+      <c r="E4" s="7"/>
+      <c r="F4" s="8"/>
+    </row>
+    <row r="5" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A5" s="37" t="s">
+        <v>30</v>
+      </c>
+      <c r="B5" s="57" t="s">
+        <v>31</v>
+      </c>
+      <c r="C5" s="58" t="s">
+        <v>32</v>
+      </c>
+      <c r="D5" s="58" t="s">
+        <v>43</v>
+      </c>
+      <c r="E5" s="60"/>
+      <c r="F5" s="62"/>
+    </row>
+    <row r="6" spans="1:7" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A6" s="37" t="s">
+        <v>30</v>
+      </c>
+      <c r="B6" s="57"/>
+      <c r="C6" s="59"/>
+      <c r="D6" s="59"/>
+      <c r="E6" s="61"/>
+      <c r="F6" s="63"/>
+    </row>
+    <row r="7" spans="1:7" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A7" s="37" t="s">
+        <v>33</v>
+      </c>
+      <c r="B7" s="38" t="s">
+        <v>34</v>
+      </c>
+      <c r="C7" s="39" t="s">
+        <v>32</v>
+      </c>
+      <c r="D7" s="39" t="s">
+        <v>43</v>
+      </c>
+      <c r="E7" s="40"/>
+      <c r="F7" s="41"/>
+    </row>
+    <row r="8" spans="1:7" ht="15.75" customHeight="1" collapsed="1" x14ac:dyDescent="0.25">
+      <c r="A8" s="42" t="s">
+        <v>35</v>
+      </c>
+      <c r="B8" s="43" t="s">
+        <v>36</v>
+      </c>
+      <c r="C8" s="44"/>
+    </row>
+    <row r="9" spans="1:7" ht="15.75" hidden="1" customHeight="1" outlineLevel="1" x14ac:dyDescent="0.25">
+      <c r="A9" s="45" t="s">
+        <v>14</v>
+      </c>
+      <c r="B9" s="46" t="s">
+        <v>37</v>
+      </c>
+      <c r="C9" s="10" t="s">
+        <v>15</v>
+      </c>
+      <c r="D9" s="11" t="s">
+        <v>16</v>
+      </c>
+      <c r="E9" s="12" t="s">
+        <v>8</v>
+      </c>
+      <c r="F9" s="12" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="10" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A10" s="34" t="s">
+        <v>12</v>
+      </c>
+      <c r="B10" t="s">
+        <v>38</v>
+      </c>
+      <c r="C10" t="s">
+        <v>39</v>
+      </c>
+      <c r="D10" t="s">
+        <v>44</v>
+      </c>
+      <c r="E10" s="47" t="s">
+        <v>20</v>
+      </c>
+      <c r="F10" s="47" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="11" spans="1:7" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A11" s="42" t="s">
+        <v>12</v>
+      </c>
+      <c r="E11" s="9"/>
+      <c r="F11" s="9"/>
+    </row>
+    <row r="12" spans="1:7" ht="24.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A12" s="48" t="s">
+        <v>5</v>
+      </c>
+      <c r="C12" s="54" t="s">
+        <v>6</v>
+      </c>
+      <c r="D12" s="55"/>
+      <c r="E12" s="55"/>
+      <c r="F12" s="56"/>
+      <c r="G12" s="4"/>
+    </row>
+    <row r="13" spans="1:7" ht="24.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A13" s="49" t="s">
+        <v>5</v>
+      </c>
+      <c r="C13" s="50" t="s">
+        <v>40</v>
+      </c>
+      <c r="D13" s="51" t="s">
+        <v>45</v>
+      </c>
+      <c r="E13" s="52" t="s">
+        <v>41</v>
+      </c>
+      <c r="F13" s="53" t="s">
+        <v>21</v>
+      </c>
+    </row>
+  </sheetData>
+  <mergeCells count="6">
+    <mergeCell ref="C12:F12"/>
+    <mergeCell ref="B5:B6"/>
+    <mergeCell ref="C5:C6"/>
+    <mergeCell ref="D5:D6"/>
+    <mergeCell ref="E5:E6"/>
+    <mergeCell ref="F5:F6"/>
+  </mergeCells>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+  <legacyDrawing r:id="rId2"/>
 </worksheet>
 </file>
</xml_diff>